<commit_message>
optimize heuristics and add more members available in data
</commit_message>
<xml_diff>
--- a/Data/Squirrel_Optimization.xlsx
+++ b/Data/Squirrel_Optimization.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quoc Minh\Documents\MyData\Gosei\squirrel_optimization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quoc Minh\Documents\MyData\Gosei\squirrel_optimization\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BF5EA6-9ACF-4F2F-A940-FF692C19F4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2E31C0-C1C2-4394-980A-6E2BA3D8CF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="480" windowWidth="21600" windowHeight="14190" firstSheet="1" activeTab="4" xr2:uid="{0EA101CE-307B-403F-950F-90B1833965F6}"/>
+    <workbookView xWindow="8175" yWindow="195" windowWidth="21600" windowHeight="14190" firstSheet="3" activeTab="5" xr2:uid="{0EA101CE-307B-403F-950F-90B1833965F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Vacancy" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,11 @@
     <sheet name="Team Member Availability" sheetId="6" r:id="rId6"/>
     <sheet name="Team Member Worksite Preference" sheetId="7" r:id="rId7"/>
     <sheet name="Team Member Shift Preference" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Team Member Measurement'!$A$1:$C$42</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="204">
   <si>
     <t>StartDate</t>
   </si>
@@ -407,127 +411,250 @@
     <t>Minimum Hours per shift</t>
   </si>
   <si>
-    <t>72700B73-0CEF-4240-873B-02ED64394BFCX</t>
-  </si>
-  <si>
-    <t>B53FC927-5B2E-4408-8BE7-08C20894C10DX</t>
-  </si>
-  <si>
-    <t>4E41E5F0-D04C-4995-BDDF-14FCC0074A40X</t>
-  </si>
-  <si>
-    <t>43C5B72F-C1D4-4F04-BD7E-158890106768X</t>
-  </si>
-  <si>
-    <t>0960C092-2944-4CED-97B2-15EED4F8E2A3X</t>
-  </si>
-  <si>
-    <t>B8CD2BAD-0C81-444D-9409-174282382D46X</t>
-  </si>
-  <si>
-    <t>D123BD71-A84E-46CC-B7BB-195CACE07E8DX</t>
-  </si>
-  <si>
-    <t>DB9AE1B1-E84B-4F51-901C-1BCF58B50E34X</t>
-  </si>
-  <si>
-    <t>64F3718F-9FD2-444B-96FD-1DCDA0C8091DX</t>
-  </si>
-  <si>
-    <t>CD34EC19-BCAB-4959-88F0-2088ED201FA8X</t>
-  </si>
-  <si>
-    <t>817FA2A4-1643-40F0-B1BA-254ED03D0A56X</t>
-  </si>
-  <si>
-    <t>6B0A4CE9-3229-432D-989A-25E5F8E7743DX</t>
-  </si>
-  <si>
-    <t>7C4FFBFE-F064-4D71-B585-29A7CED2269DX</t>
-  </si>
-  <si>
-    <t>DFD38BDE-9BFB-4265-96E7-2AA13095A616X</t>
-  </si>
-  <si>
-    <t>6CB927A1-3A91-4074-95DF-3E03DB507301X</t>
-  </si>
-  <si>
-    <t>CA1EFE53-5099-4339-AD29-3FF2D23D4F13X</t>
-  </si>
-  <si>
-    <t>F4639561-DB63-4A0D-B97C-4C50EF71C40AX</t>
-  </si>
-  <si>
-    <t>713B24EE-7B31-4267-B30F-5B6A80114E9AX</t>
-  </si>
-  <si>
-    <t>8745C5FB-A941-43BE-9473-63FE6CCA809EX</t>
-  </si>
-  <si>
-    <t>829DD9D4-C506-437E-9DE5-6E90D2053632X</t>
-  </si>
-  <si>
-    <t>26BF86A5-E6F4-47DD-99B7-77101F1CFA5AX</t>
-  </si>
-  <si>
-    <t>E5D36EB9-0D94-4374-9ADA-8E1907388840X</t>
-  </si>
-  <si>
-    <t>D9826D86-A95E-4388-BE46-90051399B297X</t>
-  </si>
-  <si>
-    <t>94C2BDDA-5E5E-4DA1-BB0F-9B988BEFF62BX</t>
-  </si>
-  <si>
-    <t>2797BD61-D136-4322-B977-A40E51A2D327X</t>
-  </si>
-  <si>
-    <t>4AC8EE58-5096-4EC5-B439-BA500B3A4156X</t>
-  </si>
-  <si>
-    <t>9CBEA724-DE2F-4C4E-9F4E-C0A1E205F2B1X</t>
-  </si>
-  <si>
-    <t>BD95C271-D6AA-47F3-8006-C0ABBED4E815X</t>
-  </si>
-  <si>
-    <t>4F140B9E-B39D-423B-8597-CAD8367387DFX</t>
-  </si>
-  <si>
-    <t>2F826996-742C-4C31-BDAA-D1A8176293EEX</t>
-  </si>
-  <si>
-    <t>F5D32F0B-5AE8-4362-B358-D543295CDC4AX</t>
-  </si>
-  <si>
-    <t>CCE6F1B0-DFCE-45BF-B2E5-D900ED20182CX</t>
-  </si>
-  <si>
-    <t>F773937D-2B29-498E-9F16-DBD6C39E327DX</t>
-  </si>
-  <si>
-    <t>4EB82AAC-4602-4DA6-9348-DDD84DEFB287X</t>
-  </si>
-  <si>
-    <t>34352998-500B-47CB-B163-E16F11B94256X</t>
-  </si>
-  <si>
-    <t>53FD97B1-8E92-4A1D-990F-F16360AD9EEAX</t>
-  </si>
-  <si>
-    <t>9673B449-5C0F-4B49-8D2B-F5AC2E6B76CCX</t>
-  </si>
-  <si>
-    <t>D90A51DA-38D4-465E-99AA-F740A04AB2E8X</t>
-  </si>
-  <si>
-    <t>92764A21-6456-432B-B126-FA53152BBC3DX</t>
-  </si>
-  <si>
-    <t>21FA0B01-4305-468A-B3B6-FC665498E929X</t>
-  </si>
-  <si>
-    <t>9C3E19DC-3666-4964-867A-FF5895F83038X</t>
+    <t>Minh A1</t>
+  </si>
+  <si>
+    <t>Minh A2</t>
+  </si>
+  <si>
+    <t>Minh A3</t>
+  </si>
+  <si>
+    <t>Minh A4</t>
+  </si>
+  <si>
+    <t>Minh A5</t>
+  </si>
+  <si>
+    <t>Minh A6</t>
+  </si>
+  <si>
+    <t>Minh A7</t>
+  </si>
+  <si>
+    <t>Minh A8</t>
+  </si>
+  <si>
+    <t>Minh A9</t>
+  </si>
+  <si>
+    <t>Minh A10</t>
+  </si>
+  <si>
+    <t>Minh A11</t>
+  </si>
+  <si>
+    <t>Minh A12</t>
+  </si>
+  <si>
+    <t>Minh A13</t>
+  </si>
+  <si>
+    <t>Minh A14</t>
+  </si>
+  <si>
+    <t>Minh A15</t>
+  </si>
+  <si>
+    <t>Minh A16</t>
+  </si>
+  <si>
+    <t>Minh A17</t>
+  </si>
+  <si>
+    <t>Minh A18</t>
+  </si>
+  <si>
+    <t>Minh A19</t>
+  </si>
+  <si>
+    <t>Minh A20</t>
+  </si>
+  <si>
+    <t>Minh A21</t>
+  </si>
+  <si>
+    <t>Minh A22</t>
+  </si>
+  <si>
+    <t>Minh A23</t>
+  </si>
+  <si>
+    <t>Minh A24</t>
+  </si>
+  <si>
+    <t>Minh A25</t>
+  </si>
+  <si>
+    <t>Minh A26</t>
+  </si>
+  <si>
+    <t>Minh A27</t>
+  </si>
+  <si>
+    <t>Minh A28</t>
+  </si>
+  <si>
+    <t>Minh A29</t>
+  </si>
+  <si>
+    <t>Minh A30</t>
+  </si>
+  <si>
+    <t>Minh A31</t>
+  </si>
+  <si>
+    <t>Minh A32</t>
+  </si>
+  <si>
+    <t>Minh A33</t>
+  </si>
+  <si>
+    <t>Minh A34</t>
+  </si>
+  <si>
+    <t>Minh A35</t>
+  </si>
+  <si>
+    <t>Minh A36</t>
+  </si>
+  <si>
+    <t>Minh A37</t>
+  </si>
+  <si>
+    <t>Minh A38</t>
+  </si>
+  <si>
+    <t>Minh A39</t>
+  </si>
+  <si>
+    <t>Minh A40</t>
+  </si>
+  <si>
+    <t>Minh A41</t>
+  </si>
+  <si>
+    <t>MINH-A1</t>
+  </si>
+  <si>
+    <t>MINH-A2</t>
+  </si>
+  <si>
+    <t>MINH-A3</t>
+  </si>
+  <si>
+    <t>MINH-A4</t>
+  </si>
+  <si>
+    <t>MINH-A5</t>
+  </si>
+  <si>
+    <t>MINH-A6</t>
+  </si>
+  <si>
+    <t>MINH-A7</t>
+  </si>
+  <si>
+    <t>MINH-A8</t>
+  </si>
+  <si>
+    <t>MINH-A9</t>
+  </si>
+  <si>
+    <t>MINH-A10</t>
+  </si>
+  <si>
+    <t>MINH-A11</t>
+  </si>
+  <si>
+    <t>MINH-A12</t>
+  </si>
+  <si>
+    <t>MINH-A13</t>
+  </si>
+  <si>
+    <t>MINH-A14</t>
+  </si>
+  <si>
+    <t>MINH-A15</t>
+  </si>
+  <si>
+    <t>MINH-A16</t>
+  </si>
+  <si>
+    <t>MINH-A17</t>
+  </si>
+  <si>
+    <t>MINH-A18</t>
+  </si>
+  <si>
+    <t>MINH-A19</t>
+  </si>
+  <si>
+    <t>MINH-A20</t>
+  </si>
+  <si>
+    <t>MINH-A21</t>
+  </si>
+  <si>
+    <t>MINH-A22</t>
+  </si>
+  <si>
+    <t>MINH-A23</t>
+  </si>
+  <si>
+    <t>MINH-A24</t>
+  </si>
+  <si>
+    <t>MINH-A25</t>
+  </si>
+  <si>
+    <t>MINH-A26</t>
+  </si>
+  <si>
+    <t>MINH-A27</t>
+  </si>
+  <si>
+    <t>MINH-A28</t>
+  </si>
+  <si>
+    <t>MINH-A29</t>
+  </si>
+  <si>
+    <t>MINH-A30</t>
+  </si>
+  <si>
+    <t>MINH-A31</t>
+  </si>
+  <si>
+    <t>MINH-A32</t>
+  </si>
+  <si>
+    <t>MINH-A33</t>
+  </si>
+  <si>
+    <t>MINH-A34</t>
+  </si>
+  <si>
+    <t>MINH-A35</t>
+  </si>
+  <si>
+    <t>MINH-A36</t>
+  </si>
+  <si>
+    <t>MINH-A37</t>
+  </si>
+  <si>
+    <t>MINH-A38</t>
+  </si>
+  <si>
+    <t>MINH-A39</t>
+  </si>
+  <si>
+    <t>MINH-A40</t>
+  </si>
+  <si>
+    <t>MINH-A41</t>
   </si>
 </sst>
 </file>
@@ -537,10 +664,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -990,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6853324-1890-466F-B02D-CC91A3DB6358}">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2456,7 +2589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED13B433-A9A4-4484-8F6E-1014F2CD242E}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -2539,13 +2672,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84EFB2CF-ABC2-425C-992C-48AA3E448ADF}">
   <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -2563,10 +2696,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -2574,10 +2707,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -2585,10 +2718,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -2596,10 +2729,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -2607,10 +2740,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -2618,10 +2751,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -2629,10 +2762,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -2640,10 +2773,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -2651,10 +2784,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -2662,10 +2795,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -2673,10 +2806,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -2684,10 +2817,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -2695,10 +2828,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -2706,10 +2839,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
@@ -2717,10 +2850,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -2728,10 +2861,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
@@ -2739,10 +2872,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -2750,10 +2883,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
@@ -2761,10 +2894,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -2772,10 +2905,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
@@ -2783,10 +2916,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -2794,10 +2927,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
@@ -2805,10 +2938,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
@@ -2816,10 +2949,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -2827,10 +2960,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
@@ -2838,10 +2971,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
@@ -2849,10 +2982,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="C28" t="s">
         <v>11</v>
@@ -2860,10 +2993,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
         <v>11</v>
@@ -2871,10 +3004,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C30" t="s">
         <v>11</v>
@@ -2882,10 +3015,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
         <v>11</v>
@@ -2893,10 +3026,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
@@ -2904,10 +3037,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
@@ -2915,10 +3048,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
         <v>11</v>
@@ -2926,10 +3059,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
@@ -2937,10 +3070,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>92</v>
+        <v>26</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
@@ -2948,10 +3081,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
         <v>11</v>
@@ -2959,10 +3092,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C38" t="s">
         <v>11</v>
@@ -2970,10 +3103,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="C39" t="s">
         <v>11</v>
@@ -2981,10 +3114,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C40" t="s">
         <v>11</v>
@@ -2992,10 +3125,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="C41" t="s">
         <v>11</v>
@@ -3003,10 +3136,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
         <v>11</v>
@@ -3014,10 +3147,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>163</v>
+      </c>
+      <c r="B43" t="s">
         <v>122</v>
-      </c>
-      <c r="B43" t="s">
-        <v>24</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
@@ -3025,10 +3158,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>164</v>
+      </c>
+      <c r="B44" t="s">
         <v>123</v>
-      </c>
-      <c r="B44" t="s">
-        <v>26</v>
       </c>
       <c r="C44" t="s">
         <v>11</v>
@@ -3036,10 +3169,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>165</v>
+      </c>
+      <c r="B45" t="s">
         <v>124</v>
-      </c>
-      <c r="B45" t="s">
-        <v>28</v>
       </c>
       <c r="C45" t="s">
         <v>11</v>
@@ -3047,10 +3180,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>166</v>
+      </c>
+      <c r="B46" t="s">
         <v>125</v>
-      </c>
-      <c r="B46" t="s">
-        <v>30</v>
       </c>
       <c r="C46" t="s">
         <v>11</v>
@@ -3058,10 +3191,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>167</v>
+      </c>
+      <c r="B47" t="s">
         <v>126</v>
-      </c>
-      <c r="B47" t="s">
-        <v>32</v>
       </c>
       <c r="C47" t="s">
         <v>11</v>
@@ -3069,10 +3202,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>168</v>
+      </c>
+      <c r="B48" t="s">
         <v>127</v>
-      </c>
-      <c r="B48" t="s">
-        <v>34</v>
       </c>
       <c r="C48" t="s">
         <v>11</v>
@@ -3080,10 +3213,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>169</v>
+      </c>
+      <c r="B49" t="s">
         <v>128</v>
-      </c>
-      <c r="B49" t="s">
-        <v>36</v>
       </c>
       <c r="C49" t="s">
         <v>11</v>
@@ -3091,10 +3224,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>170</v>
+      </c>
+      <c r="B50" t="s">
         <v>129</v>
-      </c>
-      <c r="B50" t="s">
-        <v>38</v>
       </c>
       <c r="C50" t="s">
         <v>11</v>
@@ -3102,10 +3235,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>171</v>
+      </c>
+      <c r="B51" t="s">
         <v>130</v>
-      </c>
-      <c r="B51" t="s">
-        <v>40</v>
       </c>
       <c r="C51" t="s">
         <v>11</v>
@@ -3113,10 +3246,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>172</v>
+      </c>
+      <c r="B52" t="s">
         <v>131</v>
-      </c>
-      <c r="B52" t="s">
-        <v>42</v>
       </c>
       <c r="C52" t="s">
         <v>11</v>
@@ -3124,10 +3257,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>173</v>
+      </c>
+      <c r="B53" t="s">
         <v>132</v>
-      </c>
-      <c r="B53" t="s">
-        <v>44</v>
       </c>
       <c r="C53" t="s">
         <v>11</v>
@@ -3135,10 +3268,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>174</v>
+      </c>
+      <c r="B54" t="s">
         <v>133</v>
-      </c>
-      <c r="B54" t="s">
-        <v>46</v>
       </c>
       <c r="C54" t="s">
         <v>11</v>
@@ -3146,10 +3279,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>175</v>
+      </c>
+      <c r="B55" t="s">
         <v>134</v>
-      </c>
-      <c r="B55" t="s">
-        <v>48</v>
       </c>
       <c r="C55" t="s">
         <v>11</v>
@@ -3157,10 +3290,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B56" t="s">
         <v>135</v>
-      </c>
-      <c r="B56" t="s">
-        <v>50</v>
       </c>
       <c r="C56" t="s">
         <v>11</v>
@@ -3168,10 +3301,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>177</v>
+      </c>
+      <c r="B57" t="s">
         <v>136</v>
-      </c>
-      <c r="B57" t="s">
-        <v>52</v>
       </c>
       <c r="C57" t="s">
         <v>11</v>
@@ -3179,10 +3312,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>178</v>
+      </c>
+      <c r="B58" t="s">
         <v>137</v>
-      </c>
-      <c r="B58" t="s">
-        <v>54</v>
       </c>
       <c r="C58" t="s">
         <v>11</v>
@@ -3190,10 +3323,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>179</v>
+      </c>
+      <c r="B59" t="s">
         <v>138</v>
-      </c>
-      <c r="B59" t="s">
-        <v>56</v>
       </c>
       <c r="C59" t="s">
         <v>11</v>
@@ -3201,10 +3334,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>180</v>
+      </c>
+      <c r="B60" t="s">
         <v>139</v>
-      </c>
-      <c r="B60" t="s">
-        <v>58</v>
       </c>
       <c r="C60" t="s">
         <v>11</v>
@@ -3212,10 +3345,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>181</v>
+      </c>
+      <c r="B61" t="s">
         <v>140</v>
-      </c>
-      <c r="B61" t="s">
-        <v>60</v>
       </c>
       <c r="C61" t="s">
         <v>11</v>
@@ -3223,10 +3356,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>182</v>
+      </c>
+      <c r="B62" t="s">
         <v>141</v>
-      </c>
-      <c r="B62" t="s">
-        <v>62</v>
       </c>
       <c r="C62" t="s">
         <v>11</v>
@@ -3234,10 +3367,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>183</v>
+      </c>
+      <c r="B63" t="s">
         <v>142</v>
-      </c>
-      <c r="B63" t="s">
-        <v>64</v>
       </c>
       <c r="C63" t="s">
         <v>11</v>
@@ -3245,10 +3378,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>184</v>
+      </c>
+      <c r="B64" t="s">
         <v>143</v>
-      </c>
-      <c r="B64" t="s">
-        <v>66</v>
       </c>
       <c r="C64" t="s">
         <v>11</v>
@@ -3256,10 +3389,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>185</v>
+      </c>
+      <c r="B65" t="s">
         <v>144</v>
-      </c>
-      <c r="B65" t="s">
-        <v>68</v>
       </c>
       <c r="C65" t="s">
         <v>11</v>
@@ -3267,10 +3400,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>186</v>
+      </c>
+      <c r="B66" t="s">
         <v>145</v>
-      </c>
-      <c r="B66" t="s">
-        <v>70</v>
       </c>
       <c r="C66" t="s">
         <v>11</v>
@@ -3278,10 +3411,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>187</v>
+      </c>
+      <c r="B67" t="s">
         <v>146</v>
-      </c>
-      <c r="B67" t="s">
-        <v>72</v>
       </c>
       <c r="C67" t="s">
         <v>11</v>
@@ -3289,10 +3422,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>188</v>
+      </c>
+      <c r="B68" t="s">
         <v>147</v>
-      </c>
-      <c r="B68" t="s">
-        <v>74</v>
       </c>
       <c r="C68" t="s">
         <v>11</v>
@@ -3300,10 +3433,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>189</v>
+      </c>
+      <c r="B69" t="s">
         <v>148</v>
-      </c>
-      <c r="B69" t="s">
-        <v>76</v>
       </c>
       <c r="C69" t="s">
         <v>11</v>
@@ -3311,10 +3444,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>190</v>
+      </c>
+      <c r="B70" t="s">
         <v>149</v>
-      </c>
-      <c r="B70" t="s">
-        <v>78</v>
       </c>
       <c r="C70" t="s">
         <v>11</v>
@@ -3322,10 +3455,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>191</v>
+      </c>
+      <c r="B71" t="s">
         <v>150</v>
-      </c>
-      <c r="B71" t="s">
-        <v>80</v>
       </c>
       <c r="C71" t="s">
         <v>11</v>
@@ -3333,10 +3466,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>192</v>
+      </c>
+      <c r="B72" t="s">
         <v>151</v>
-      </c>
-      <c r="B72" t="s">
-        <v>82</v>
       </c>
       <c r="C72" t="s">
         <v>11</v>
@@ -3344,10 +3477,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>193</v>
+      </c>
+      <c r="B73" t="s">
         <v>152</v>
-      </c>
-      <c r="B73" t="s">
-        <v>84</v>
       </c>
       <c r="C73" t="s">
         <v>11</v>
@@ -3355,10 +3488,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>194</v>
+      </c>
+      <c r="B74" t="s">
         <v>153</v>
-      </c>
-      <c r="B74" t="s">
-        <v>86</v>
       </c>
       <c r="C74" t="s">
         <v>11</v>
@@ -3366,10 +3499,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>195</v>
+      </c>
+      <c r="B75" t="s">
         <v>154</v>
-      </c>
-      <c r="B75" t="s">
-        <v>88</v>
       </c>
       <c r="C75" t="s">
         <v>11</v>
@@ -3377,10 +3510,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>196</v>
+      </c>
+      <c r="B76" t="s">
         <v>155</v>
-      </c>
-      <c r="B76" t="s">
-        <v>90</v>
       </c>
       <c r="C76" t="s">
         <v>11</v>
@@ -3388,10 +3521,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>197</v>
+      </c>
+      <c r="B77" t="s">
         <v>156</v>
-      </c>
-      <c r="B77" t="s">
-        <v>92</v>
       </c>
       <c r="C77" t="s">
         <v>11</v>
@@ -3399,10 +3532,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>198</v>
+      </c>
+      <c r="B78" t="s">
         <v>157</v>
-      </c>
-      <c r="B78" t="s">
-        <v>94</v>
       </c>
       <c r="C78" t="s">
         <v>11</v>
@@ -3410,10 +3543,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>199</v>
+      </c>
+      <c r="B79" t="s">
         <v>158</v>
-      </c>
-      <c r="B79" t="s">
-        <v>96</v>
       </c>
       <c r="C79" t="s">
         <v>11</v>
@@ -3421,10 +3554,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>200</v>
+      </c>
+      <c r="B80" t="s">
         <v>159</v>
-      </c>
-      <c r="B80" t="s">
-        <v>98</v>
       </c>
       <c r="C80" t="s">
         <v>11</v>
@@ -3432,10 +3565,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>201</v>
+      </c>
+      <c r="B81" t="s">
         <v>160</v>
-      </c>
-      <c r="B81" t="s">
-        <v>100</v>
       </c>
       <c r="C81" t="s">
         <v>11</v>
@@ -3443,10 +3576,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>202</v>
+      </c>
+      <c r="B82" t="s">
         <v>161</v>
-      </c>
-      <c r="B82" t="s">
-        <v>102</v>
       </c>
       <c r="C82" t="s">
         <v>11</v>
@@ -3454,30 +3587,38 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>203</v>
+      </c>
+      <c r="B83" t="s">
         <v>162</v>
       </c>
-      <c r="B83" t="s">
-        <v>104</v>
-      </c>
       <c r="C83" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C42" xr:uid="{84EFB2CF-ABC2-425C-992C-48AA3E448ADF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C42">
+      <sortCondition ref="B1:B42"/>
+    </sortState>
+  </autoFilter>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46FED855-9E45-4643-B273-1083C4F3A277}">
-  <dimension ref="A1:D135"/>
+  <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="46.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
     <col min="3" max="4" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3497,10 +3638,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>163</v>
       </c>
       <c r="C2" s="2">
         <v>44564</v>
@@ -3511,10 +3652,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>164</v>
       </c>
       <c r="C3" s="2">
         <v>44564</v>
@@ -3525,10 +3666,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>165</v>
       </c>
       <c r="C4" s="2">
         <v>44564</v>
@@ -3539,10 +3680,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>166</v>
       </c>
       <c r="C5" s="2">
         <v>44564</v>
@@ -3553,10 +3694,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="C6" s="2">
         <v>44564</v>
@@ -3567,10 +3708,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2">
         <v>44564</v>
@@ -3581,10 +3722,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2">
         <v>44564</v>
@@ -3595,10 +3736,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2">
         <v>44564</v>
@@ -3609,10 +3750,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="C10" s="2">
         <v>44564</v>
@@ -3623,66 +3764,66 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="C11" s="2">
-        <v>44564.166666666664</v>
+        <v>44564</v>
       </c>
       <c r="D11" s="2">
-        <v>44564.75</v>
+        <v>44565</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="C12" s="2">
-        <v>44564.166666666664</v>
+        <v>44564</v>
       </c>
       <c r="D12" s="2">
-        <v>44564.75</v>
+        <v>44565</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="C13" s="2">
-        <v>44564.166666666664</v>
+        <v>44564</v>
       </c>
       <c r="D13" s="2">
-        <v>44564.75</v>
+        <v>44565</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C14" s="2">
-        <v>44564.166666666664</v>
+        <v>44564</v>
       </c>
       <c r="D14" s="2">
-        <v>44564.75</v>
+        <v>44565</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C15" s="2">
         <v>44564.166666666664</v>
@@ -3693,10 +3834,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="C16" s="2">
         <v>44564.166666666664</v>
@@ -3707,10 +3848,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C17" s="2">
         <v>44564.166666666664</v>
@@ -3721,66 +3862,66 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="C18" s="2">
-        <v>44565</v>
+        <v>44564.166666666664</v>
       </c>
       <c r="D18" s="2">
-        <v>44566</v>
+        <v>44564.75</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="C19" s="2">
-        <v>44565</v>
+        <v>44564.166666666664</v>
       </c>
       <c r="D19" s="2">
-        <v>44566</v>
+        <v>44564.75</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C20" s="2">
-        <v>44565</v>
+        <v>44564.166666666664</v>
       </c>
       <c r="D20" s="2">
-        <v>44566</v>
+        <v>44564.75</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="C21" s="2">
-        <v>44565</v>
+        <v>44564.166666666664</v>
       </c>
       <c r="D21" s="2">
-        <v>44566</v>
+        <v>44564.75</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C22" s="2">
         <v>44565</v>
@@ -3791,10 +3932,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="C23" s="2">
         <v>44565</v>
@@ -3805,10 +3946,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C24" s="2">
         <v>44565</v>
@@ -3819,10 +3960,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C25" s="2">
         <v>44565</v>
@@ -3833,10 +3974,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="C26" s="2">
         <v>44565</v>
@@ -3847,66 +3988,66 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C27" s="2">
-        <v>44565.166666666664</v>
+        <v>44565</v>
       </c>
       <c r="D27" s="2">
-        <v>44565.75</v>
+        <v>44566</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>34</v>
       </c>
       <c r="C28" s="2">
-        <v>44565.166666666664</v>
+        <v>44565</v>
       </c>
       <c r="D28" s="2">
-        <v>44565.75</v>
+        <v>44566</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C29" s="2">
-        <v>44565.166666666664</v>
+        <v>44565</v>
       </c>
       <c r="D29" s="2">
-        <v>44565.75</v>
+        <v>44566</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="C30" s="2">
-        <v>44565.166666666664</v>
+        <v>44565</v>
       </c>
       <c r="D30" s="2">
-        <v>44565.75</v>
+        <v>44566</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="C31" s="2">
         <v>44565.166666666664</v>
@@ -3917,10 +4058,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="C32" s="2">
         <v>44565.166666666664</v>
@@ -3931,10 +4072,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C33" s="2">
         <v>44565.166666666664</v>
@@ -3945,66 +4086,66 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="C34" s="2">
-        <v>44566</v>
+        <v>44565.166666666664</v>
       </c>
       <c r="D34" s="2">
-        <v>44567</v>
+        <v>44565.75</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="C35" s="2">
-        <v>44566</v>
+        <v>44565.166666666664</v>
       </c>
       <c r="D35" s="2">
-        <v>44567</v>
+        <v>44565.75</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="C36" s="2">
-        <v>44566</v>
+        <v>44565.166666666664</v>
       </c>
       <c r="D36" s="2">
-        <v>44567</v>
+        <v>44565.75</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C37" s="2">
-        <v>44566</v>
+        <v>44565.166666666664</v>
       </c>
       <c r="D37" s="2">
-        <v>44567</v>
+        <v>44565.75</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C38" s="2">
         <v>44566</v>
@@ -4015,10 +4156,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>27</v>
       </c>
       <c r="B39" t="s">
-        <v>104</v>
+        <v>28</v>
       </c>
       <c r="C39" s="2">
         <v>44566</v>
@@ -4029,10 +4170,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C40" s="2">
         <v>44566</v>
@@ -4043,10 +4184,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="C41" s="2">
         <v>44566</v>
@@ -4057,10 +4198,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C42" s="2">
         <v>44566</v>
@@ -4071,66 +4212,66 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C43" s="2">
-        <v>44566.166666666664</v>
+        <v>44566</v>
       </c>
       <c r="D43" s="2">
-        <v>44566.75</v>
+        <v>44567</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
       <c r="C44" s="2">
-        <v>44566.166666666664</v>
+        <v>44566</v>
       </c>
       <c r="D44" s="2">
-        <v>44566.75</v>
+        <v>44567</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="C45" s="2">
-        <v>44566.166666666664</v>
+        <v>44566</v>
       </c>
       <c r="D45" s="2">
-        <v>44566.75</v>
+        <v>44567</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B46" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C46" s="2">
-        <v>44566.166666666664</v>
+        <v>44566</v>
       </c>
       <c r="D46" s="2">
-        <v>44566.75</v>
+        <v>44567</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C47" s="2">
         <v>44566.166666666664</v>
@@ -4141,10 +4282,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B48" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="C48" s="2">
         <v>44566.166666666664</v>
@@ -4155,10 +4296,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B49" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C49" s="2">
         <v>44566.166666666664</v>
@@ -4169,66 +4310,66 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C50" s="2">
-        <v>44567</v>
+        <v>44566.166666666664</v>
       </c>
       <c r="D50" s="2">
-        <v>44568</v>
+        <v>44566.75</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="C51" s="2">
-        <v>44567</v>
+        <v>44566.166666666664</v>
       </c>
       <c r="D51" s="2">
-        <v>44568</v>
+        <v>44566.75</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="B52" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="C52" s="2">
-        <v>44567</v>
+        <v>44566.166666666664</v>
       </c>
       <c r="D52" s="2">
-        <v>44568</v>
+        <v>44566.75</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>104</v>
+        <v>56</v>
       </c>
       <c r="C53" s="2">
-        <v>44567</v>
+        <v>44566.166666666664</v>
       </c>
       <c r="D53" s="2">
-        <v>44568</v>
+        <v>44566.75</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B54" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C54" s="2">
         <v>44567</v>
@@ -4239,10 +4380,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C55" s="2">
         <v>44567</v>
@@ -4253,10 +4394,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B56" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C56" s="2">
         <v>44567</v>
@@ -4267,10 +4408,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="B57" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="C57" s="2">
         <v>44567</v>
@@ -4281,10 +4422,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C58" s="2">
         <v>44567</v>
@@ -4295,66 +4436,66 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B59" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="C59" s="2">
-        <v>44567.583333333336</v>
+        <v>44567</v>
       </c>
       <c r="D59" s="2">
-        <v>44567.916666666664</v>
+        <v>44568</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="B60" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="C60" s="2">
-        <v>44567.583333333336</v>
+        <v>44567</v>
       </c>
       <c r="D60" s="2">
-        <v>44567.916666666664</v>
+        <v>44568</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="B61" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="C61" s="2">
-        <v>44567.583333333336</v>
+        <v>44567</v>
       </c>
       <c r="D61" s="2">
-        <v>44567.916666666664</v>
+        <v>44568</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="C62" s="2">
-        <v>44567.583333333336</v>
+        <v>44567</v>
       </c>
       <c r="D62" s="2">
-        <v>44567.916666666664</v>
+        <v>44568</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="B63" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="C63" s="2">
         <v>44567.583333333336</v>
@@ -4365,10 +4506,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B64" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C64" s="2">
         <v>44567.583333333336</v>
@@ -4379,10 +4520,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="B65" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="C65" s="2">
         <v>44567.583333333336</v>
@@ -4393,10 +4534,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B66" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="C66" s="2">
         <v>44567.583333333336</v>
@@ -4407,10 +4548,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="B67" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="C67" s="2">
         <v>44567.583333333336</v>
@@ -4421,10 +4562,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="B68" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="C68" s="2">
         <v>44567.583333333336</v>
@@ -4435,66 +4576,66 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B69" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C69" s="2">
-        <v>44568</v>
+        <v>44567.583333333336</v>
       </c>
       <c r="D69" s="2">
-        <v>44569</v>
+        <v>44567.916666666664</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="B70" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="C70" s="2">
-        <v>44568</v>
+        <v>44567.583333333336</v>
       </c>
       <c r="D70" s="2">
-        <v>44569</v>
+        <v>44567.916666666664</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B71" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C71" s="2">
-        <v>44568</v>
+        <v>44567.583333333336</v>
       </c>
       <c r="D71" s="2">
-        <v>44569</v>
+        <v>44567.916666666664</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="B72" t="s">
-        <v>104</v>
+        <v>54</v>
       </c>
       <c r="C72" s="2">
-        <v>44568</v>
+        <v>44567.583333333336</v>
       </c>
       <c r="D72" s="2">
-        <v>44569</v>
+        <v>44567.916666666664</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="B73" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C73" s="2">
         <v>44568</v>
@@ -4505,10 +4646,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="B74" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="C74" s="2">
         <v>44568</v>
@@ -4519,10 +4660,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B75" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C75" s="2">
         <v>44568</v>
@@ -4533,10 +4674,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
       <c r="B76" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="C76" s="2">
         <v>44568</v>
@@ -4547,10 +4688,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="B77" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="C77" s="2">
         <v>44568</v>
@@ -4561,66 +4702,66 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="B78" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="C78" s="2">
-        <v>44568.583333333336</v>
+        <v>44568</v>
       </c>
       <c r="D78" s="2">
-        <v>44568.916666666664</v>
+        <v>44569</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B79" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C79" s="2">
-        <v>44568.583333333336</v>
+        <v>44568</v>
       </c>
       <c r="D79" s="2">
-        <v>44568.916666666664</v>
+        <v>44569</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="B80" t="s">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="C80" s="2">
-        <v>44568.583333333336</v>
+        <v>44568</v>
       </c>
       <c r="D80" s="2">
-        <v>44568.916666666664</v>
+        <v>44569</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="B81" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="C81" s="2">
-        <v>44568.583333333336</v>
+        <v>44568</v>
       </c>
       <c r="D81" s="2">
-        <v>44568.916666666664</v>
+        <v>44569</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="B82" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="C82" s="2">
         <v>44568.583333333336</v>
@@ -4631,10 +4772,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B83" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C83" s="2">
         <v>44568.583333333336</v>
@@ -4645,10 +4786,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="B84" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="C84" s="2">
         <v>44568.583333333336</v>
@@ -4659,10 +4800,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B85" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C85" s="2">
         <v>44568.583333333336</v>
@@ -4673,10 +4814,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="B86" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="C86" s="2">
         <v>44568.583333333336</v>
@@ -4687,10 +4828,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="B87" t="s">
-        <v>102</v>
+        <v>40</v>
       </c>
       <c r="C87" s="2">
         <v>44568.583333333336</v>
@@ -4701,66 +4842,66 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B88" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C88" s="2">
-        <v>44569</v>
+        <v>44568.583333333336</v>
       </c>
       <c r="D88" s="2">
-        <v>44570</v>
+        <v>44568.916666666664</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="B89" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="C89" s="2">
-        <v>44569</v>
+        <v>44568.583333333336</v>
       </c>
       <c r="D89" s="2">
-        <v>44570</v>
+        <v>44568.916666666664</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="B90" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="C90" s="2">
-        <v>44569</v>
+        <v>44568.583333333336</v>
       </c>
       <c r="D90" s="2">
-        <v>44570</v>
+        <v>44568.916666666664</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="B91" t="s">
-        <v>28</v>
+        <v>102</v>
       </c>
       <c r="C91" s="2">
-        <v>44569</v>
+        <v>44568.583333333336</v>
       </c>
       <c r="D91" s="2">
-        <v>44570</v>
+        <v>44568.916666666664</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B92" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="C92" s="2">
         <v>44569</v>
@@ -4771,10 +4912,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="B93" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="C93" s="2">
         <v>44569</v>
@@ -4785,10 +4926,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="B94" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="C94" s="2">
         <v>44569</v>
@@ -4799,10 +4940,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>103</v>
+        <v>27</v>
       </c>
       <c r="B95" t="s">
-        <v>104</v>
+        <v>28</v>
       </c>
       <c r="C95" s="2">
         <v>44569</v>
@@ -4813,10 +4954,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B96" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C96" s="2">
         <v>44569</v>
@@ -4827,66 +4968,66 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="B97" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C97" s="2">
-        <v>44569.416666666664</v>
+        <v>44569</v>
       </c>
       <c r="D97" s="2">
-        <v>44569.833333333336</v>
+        <v>44570</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="B98" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="C98" s="2">
-        <v>44569.416666666664</v>
+        <v>44569</v>
       </c>
       <c r="D98" s="2">
-        <v>44569.833333333336</v>
+        <v>44570</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="B99" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="C99" s="2">
-        <v>44569.416666666664</v>
+        <v>44569</v>
       </c>
       <c r="D99" s="2">
-        <v>44569.833333333336</v>
+        <v>44570</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B100" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C100" s="2">
-        <v>44569.416666666664</v>
+        <v>44569</v>
       </c>
       <c r="D100" s="2">
-        <v>44569.833333333336</v>
+        <v>44570</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>87</v>
+        <v>41</v>
       </c>
       <c r="B101" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="C101" s="2">
         <v>44569.416666666664</v>
@@ -4897,10 +5038,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B102" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C102" s="2">
         <v>44569.416666666664</v>
@@ -4911,10 +5052,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="B103" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="C103" s="2">
         <v>44569.416666666664</v>
@@ -4925,10 +5066,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="B104" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="C104" s="2">
         <v>44569.416666666664</v>
@@ -4939,10 +5080,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="B105" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="C105" s="2">
         <v>44569.416666666664</v>
@@ -4953,10 +5094,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="B106" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="C106" s="2">
         <v>44569.416666666664</v>
@@ -4967,66 +5108,66 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="B107" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C107" s="2">
-        <v>44569.583333333336</v>
+        <v>44569.416666666664</v>
       </c>
       <c r="D107" s="2">
-        <v>44569.916666666664</v>
+        <v>44569.833333333336</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="B108" t="s">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="C108" s="2">
-        <v>44569.583333333336</v>
+        <v>44569.416666666664</v>
       </c>
       <c r="D108" s="2">
-        <v>44569.916666666664</v>
+        <v>44569.833333333336</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="B109" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="C109" s="2">
-        <v>44569.583333333336</v>
+        <v>44569.416666666664</v>
       </c>
       <c r="D109" s="2">
-        <v>44569.916666666664</v>
+        <v>44569.833333333336</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B110" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="C110" s="2">
-        <v>44569.583333333336</v>
+        <v>44569.416666666664</v>
       </c>
       <c r="D110" s="2">
-        <v>44569.916666666664</v>
+        <v>44569.833333333336</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B111" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C111" s="2">
         <v>44569.583333333336</v>
@@ -5037,10 +5178,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B112" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C112" s="2">
         <v>44569.583333333336</v>
@@ -5051,10 +5192,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B113" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C113" s="2">
         <v>44569.583333333336</v>
@@ -5065,10 +5206,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="B114" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="C114" s="2">
         <v>44569.583333333336</v>
@@ -5079,10 +5220,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B115" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C115" s="2">
         <v>44569.583333333336</v>
@@ -5093,10 +5234,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="B116" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="C116" s="2">
         <v>44569.583333333336</v>
@@ -5107,66 +5248,66 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="B117" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="C117" s="2">
-        <v>44570</v>
+        <v>44569.583333333336</v>
       </c>
       <c r="D117" s="2">
-        <v>44571</v>
+        <v>44569.916666666664</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B118" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="C118" s="2">
-        <v>44570</v>
+        <v>44569.583333333336</v>
       </c>
       <c r="D118" s="2">
-        <v>44571</v>
+        <v>44569.916666666664</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B119" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C119" s="2">
-        <v>44570</v>
+        <v>44569.583333333336</v>
       </c>
       <c r="D119" s="2">
-        <v>44571</v>
+        <v>44569.916666666664</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B120" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C120" s="2">
-        <v>44570</v>
+        <v>44569.583333333336</v>
       </c>
       <c r="D120" s="2">
-        <v>44571</v>
+        <v>44569.916666666664</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B121" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C121" s="2">
         <v>44570</v>
@@ -5177,10 +5318,10 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="B122" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="C122" s="2">
         <v>44570</v>
@@ -5191,10 +5332,10 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B123" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C123" s="2">
         <v>44570</v>
@@ -5205,10 +5346,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="B124" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="C124" s="2">
         <v>44570</v>
@@ -5219,10 +5360,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B125" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C125" s="2">
         <v>44570</v>
@@ -5233,66 +5374,66 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B126" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="C126" s="2">
-        <v>44570.416666666664</v>
+        <v>44570</v>
       </c>
       <c r="D126" s="2">
-        <v>44570.833333333336</v>
+        <v>44571</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="B127" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C127" s="2">
-        <v>44570.416666666664</v>
+        <v>44570</v>
       </c>
       <c r="D127" s="2">
-        <v>44570.833333333336</v>
+        <v>44571</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B128" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C128" s="2">
-        <v>44570.416666666664</v>
+        <v>44570</v>
       </c>
       <c r="D128" s="2">
-        <v>44570.833333333336</v>
+        <v>44571</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B129" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C129" s="2">
-        <v>44570.416666666664</v>
+        <v>44570</v>
       </c>
       <c r="D129" s="2">
-        <v>44570.833333333336</v>
+        <v>44571</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="B130" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="C130" s="2">
         <v>44570.416666666664</v>
@@ -5303,10 +5444,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B131" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C131" s="2">
         <v>44570.416666666664</v>
@@ -5317,10 +5458,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B132" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C132" s="2">
         <v>44570.416666666664</v>
@@ -5331,10 +5472,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="B133" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C133" s="2">
         <v>44570.416666666664</v>
@@ -5345,10 +5486,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="B134" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="C134" s="2">
         <v>44570.416666666664</v>
@@ -5359,10 +5500,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B135" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C135" s="2">
         <v>44570.416666666664</v>
@@ -5371,7 +5512,64 @@
         <v>44570.833333333336</v>
       </c>
     </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>69</v>
+      </c>
+      <c r="B136" t="s">
+        <v>70</v>
+      </c>
+      <c r="C136" s="2">
+        <v>44570.416666666664</v>
+      </c>
+      <c r="D136" s="2">
+        <v>44570.833333333336</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>67</v>
+      </c>
+      <c r="B137" t="s">
+        <v>68</v>
+      </c>
+      <c r="C137" s="2">
+        <v>44570.416666666664</v>
+      </c>
+      <c r="D137" s="2">
+        <v>44570.833333333336</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>57</v>
+      </c>
+      <c r="B138" t="s">
+        <v>58</v>
+      </c>
+      <c r="C138" s="2">
+        <v>44570.416666666664</v>
+      </c>
+      <c r="D138" s="2">
+        <v>44570.833333333336</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>29</v>
+      </c>
+      <c r="B139" t="s">
+        <v>30</v>
+      </c>
+      <c r="C139" s="2">
+        <v>44570.416666666664</v>
+      </c>
+      <c r="D139" s="2">
+        <v>44570.833333333336</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5440,7 +5638,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5553,4 +5751,629 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{706BEBC1-DD6F-4EB7-A6A8-EA686A7FE5AA}">
+  <dimension ref="A10:D66"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:E66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="42.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C10" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D10" s="2">
+        <v>44565</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D11" s="2">
+        <v>44565</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D12" s="2">
+        <v>44565</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D13" s="2">
+        <v>44565</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D14" s="2">
+        <v>44565</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D15" s="2">
+        <v>44565</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D16" s="2">
+        <v>44565</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D17" s="2">
+        <v>44565</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D18" s="2">
+        <v>44565</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D19" s="2">
+        <v>44565</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D20" s="2">
+        <v>44565</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D21" s="2">
+        <v>44565</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>175</v>
+      </c>
+      <c r="C22" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D22" s="2">
+        <v>44565</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>176</v>
+      </c>
+      <c r="C23" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D23" s="2">
+        <v>44565</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>163</v>
+      </c>
+      <c r="B26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>164</v>
+      </c>
+      <c r="B27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>165</v>
+      </c>
+      <c r="B28" t="s">
+        <v>124</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>166</v>
+      </c>
+      <c r="B29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>167</v>
+      </c>
+      <c r="B30" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>168</v>
+      </c>
+      <c r="B31" t="s">
+        <v>127</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>169</v>
+      </c>
+      <c r="B32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>170</v>
+      </c>
+      <c r="B33" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>171</v>
+      </c>
+      <c r="B34" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>172</v>
+      </c>
+      <c r="B35" t="s">
+        <v>131</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>174</v>
+      </c>
+      <c r="B37" t="s">
+        <v>133</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>175</v>
+      </c>
+      <c r="B38" t="s">
+        <v>134</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>176</v>
+      </c>
+      <c r="B39" t="s">
+        <v>135</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41" t="s">
+        <v>137</v>
+      </c>
+      <c r="C41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>179</v>
+      </c>
+      <c r="B42" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>180</v>
+      </c>
+      <c r="B43" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>181</v>
+      </c>
+      <c r="B44" t="s">
+        <v>140</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>182</v>
+      </c>
+      <c r="B45" t="s">
+        <v>141</v>
+      </c>
+      <c r="C45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>183</v>
+      </c>
+      <c r="B46" t="s">
+        <v>142</v>
+      </c>
+      <c r="C46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>184</v>
+      </c>
+      <c r="B47" t="s">
+        <v>143</v>
+      </c>
+      <c r="C47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>185</v>
+      </c>
+      <c r="B48" t="s">
+        <v>144</v>
+      </c>
+      <c r="C48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>186</v>
+      </c>
+      <c r="B49" t="s">
+        <v>145</v>
+      </c>
+      <c r="C49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>187</v>
+      </c>
+      <c r="B50" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>188</v>
+      </c>
+      <c r="B51" t="s">
+        <v>147</v>
+      </c>
+      <c r="C51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>189</v>
+      </c>
+      <c r="B52" t="s">
+        <v>148</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>190</v>
+      </c>
+      <c r="B53" t="s">
+        <v>149</v>
+      </c>
+      <c r="C53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>191</v>
+      </c>
+      <c r="B54" t="s">
+        <v>150</v>
+      </c>
+      <c r="C54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>192</v>
+      </c>
+      <c r="B55" t="s">
+        <v>151</v>
+      </c>
+      <c r="C55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>193</v>
+      </c>
+      <c r="B56" t="s">
+        <v>152</v>
+      </c>
+      <c r="C56" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>194</v>
+      </c>
+      <c r="B57" t="s">
+        <v>153</v>
+      </c>
+      <c r="C57" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>195</v>
+      </c>
+      <c r="B58" t="s">
+        <v>154</v>
+      </c>
+      <c r="C58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>196</v>
+      </c>
+      <c r="B59" t="s">
+        <v>155</v>
+      </c>
+      <c r="C59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>197</v>
+      </c>
+      <c r="B60" t="s">
+        <v>156</v>
+      </c>
+      <c r="C60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>198</v>
+      </c>
+      <c r="B61" t="s">
+        <v>157</v>
+      </c>
+      <c r="C61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>199</v>
+      </c>
+      <c r="B62" t="s">
+        <v>158</v>
+      </c>
+      <c r="C62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>200</v>
+      </c>
+      <c r="B63" t="s">
+        <v>159</v>
+      </c>
+      <c r="C63" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>201</v>
+      </c>
+      <c r="B64" t="s">
+        <v>160</v>
+      </c>
+      <c r="C64" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>202</v>
+      </c>
+      <c r="B65" t="s">
+        <v>161</v>
+      </c>
+      <c r="C65" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>203</v>
+      </c>
+      <c r="B66" t="s">
+        <v>162</v>
+      </c>
+      <c r="C66" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>